<commit_message>
add functions and modify some scripts
</commit_message>
<xml_diff>
--- a/특근매식비장부.xlsx
+++ b/특근매식비장부.xlsx
@@ -103,10 +103,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>황우식, 홍춘식, 양해선, 고경수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>박지현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -283,11 +279,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>진진미, 김영애, 황은아, 성산성, 김문정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>현승호, 안명돈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>황우식, 홍춘식, 양혜선, 고경수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>진진미, 김영애, 황은하, 성찬성, 김문정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -742,7 +742,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -764,7 +764,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="3">
         <v>8000</v>
@@ -775,7 +775,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="3">
         <v>8000</v>
@@ -803,18 +803,18 @@
         <v>32000</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="3">
         <v>7000</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -825,18 +825,18 @@
         <v>16000</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3">
         <v>8000</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -847,12 +847,13 @@
         <v>7000</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -889,7 +890,7 @@
         <v>32000</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -900,7 +901,7 @@
         <v>16000</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -911,7 +912,7 @@
         <v>8000</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -953,18 +954,18 @@
         <v>16000</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2">
         <v>8000</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -978,7 +979,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1000,35 +1001,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2">
         <v>16000</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2">
         <v>8000</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2">
         <v>6550</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1039,7 +1040,7 @@
         <v>16000</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1050,7 +1051,7 @@
         <v>16000</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1072,7 +1073,7 @@
         <v>8000</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1083,7 +1084,7 @@
         <v>7800</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1094,23 +1095,23 @@
         <v>8000</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="2">
         <v>8000</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" s="2">
         <v>7400</v>
@@ -1121,13 +1122,13 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="2">
         <v>7250</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1138,7 +1139,7 @@
         <v>23550</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1160,51 +1161,51 @@
         <v>16000</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17" s="2">
         <v>12650</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" s="2">
         <v>8000</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2">
         <v>24000</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="2">
         <v>8000</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1215,7 +1216,7 @@
         <v>15650</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -1226,7 +1227,7 @@
         <v>8000</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -1237,73 +1238,73 @@
         <v>8000</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" s="2">
         <v>7800</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" s="2">
         <v>7900</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="2">
         <v>7800</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="2">
         <v>47760</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="2">
         <v>7800</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="2">
         <v>7300</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1314,7 +1315,7 @@
         <v>7700</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1325,34 +1326,34 @@
         <v>32000</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32" s="2">
         <v>7800</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B33" s="2">
         <v>8000</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B34" s="2">
         <v>7600</v>
@@ -1372,7 +1373,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1394,13 +1395,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2">
         <v>32000</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1411,7 +1412,7 @@
         <v>16000</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1422,7 +1423,7 @@
         <v>16000</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1433,7 +1434,7 @@
         <v>16000</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1444,23 +1445,23 @@
         <v>16000</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2">
         <v>40000</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2">
         <v>8000</v>
@@ -1477,29 +1478,29 @@
         <v>16000</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2">
         <v>16000</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2">
         <v>16000</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>